<commit_message>
Created JS to add HTML!!!!
</commit_message>
<xml_diff>
--- a/Javascript Bootcamp Hours.xlsx
+++ b/Javascript Bootcamp Hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP EliteBook 8470p\Documents\Coding\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34234F7-7851-4FA8-973F-1F65176D254A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF72AA5-D27D-4EB7-9DB1-B13EF6EE18B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{176BBFA2-C1D9-4FD8-8B03-D771EE46934D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
   <si>
     <t>Thursday</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Cannelle Total Hours</t>
+  </si>
+  <si>
+    <t>tues</t>
+  </si>
+  <si>
+    <t>JS LOOP</t>
   </si>
 </sst>
 </file>
@@ -765,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA44BCE-BEAF-4B71-919F-0CAAC8D672FA}">
   <dimension ref="A5:S298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R178" sqref="Q178:R178"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,147 +3451,237 @@
       </c>
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B187" s="29">
+        <v>43837</v>
+      </c>
+      <c r="C187" s="13">
+        <v>0.81527777777777777</v>
+      </c>
+      <c r="D187" s="13">
+        <v>0.83680555555555547</v>
+      </c>
       <c r="E187" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>30.99999999999989</v>
       </c>
       <c r="G187" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H187" s="28">
         <f>SUM(E187:E199)</f>
-        <v>0</v>
+        <v>-967</v>
       </c>
       <c r="J187" s="30">
         <f>(QUOTIENT(H187,60))</f>
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="K187" s="31">
         <f>MOD(H187,60)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C188" s="13">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D188" s="13">
+        <v>0.86249999999999993</v>
+      </c>
       <c r="E188" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11.999999999999957</v>
       </c>
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C189" s="13">
+        <v>0.86875000000000002</v>
+      </c>
+      <c r="D189" s="13">
+        <v>0.87986111111111109</v>
+      </c>
       <c r="E189" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>15.999999999999943</v>
       </c>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C190" s="13">
+        <v>0.8847222222222223</v>
+      </c>
+      <c r="D190" s="13">
+        <v>0.88750000000000007</v>
+      </c>
       <c r="E190" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.9999999999999858</v>
       </c>
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C191" s="13">
+        <v>0.8930555555555556</v>
+      </c>
+      <c r="D191" s="13">
+        <v>0.91805555555555562</v>
+      </c>
       <c r="E191" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>36.000000000000028</v>
       </c>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C192" s="13">
+        <v>0.97638888888888886</v>
+      </c>
+      <c r="D192" s="13">
+        <v>0.98055555555555562</v>
+      </c>
       <c r="E192" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+        <v>6.0000000000001386</v>
+      </c>
+    </row>
+    <row r="193" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C193" s="13">
+        <v>0.9868055555555556</v>
+      </c>
+      <c r="D193" s="13">
+        <v>0.99930555555555556</v>
+      </c>
       <c r="E193" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+        <v>17.999999999999936</v>
+      </c>
+    </row>
+    <row r="194" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C194" s="13">
+        <v>0</v>
+      </c>
+      <c r="D194" s="13">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E194" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="195" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C195" s="13">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D195" s="13">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="E195" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="196" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E196" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B197" s="29">
+        <v>43838</v>
+      </c>
+      <c r="C197" s="13">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D197" s="13">
+        <v>0.86597222222222225</v>
+      </c>
       <c r="E197" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+        <v>17.000000000000099</v>
+      </c>
+      <c r="G197" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H197" s="28">
+        <f>SUM(E197:E209)</f>
+        <v>-1230</v>
+      </c>
+      <c r="J197" s="30">
+        <f>(QUOTIENT(H197,60))</f>
+        <v>-20</v>
+      </c>
+      <c r="K197" s="31">
+        <f>MOD(H197,60)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="198" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B198" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C198" s="13">
+        <v>0.86597222222222225</v>
+      </c>
       <c r="E198" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+        <v>-1247</v>
+      </c>
+    </row>
+    <row r="199" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E199" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E200" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E201" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E202" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E203" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E204" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E205" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E206" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E207" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E208" s="16">
         <f t="shared" si="5"/>
         <v>0</v>

</xml_diff>

<commit_message>
Create regex for Book Tree CSV
</commit_message>
<xml_diff>
--- a/Javascript Bootcamp Hours.xlsx
+++ b/Javascript Bootcamp Hours.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP EliteBook 8470p\Documents\Coding\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB20B1DE-21C4-4105-B4AC-3482EB1BAB0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CADFE58-7882-4342-B516-AB61146781A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{176BBFA2-C1D9-4FD8-8B03-D771EE46934D}"/>
+    <workbookView xWindow="900" yWindow="1005" windowWidth="20595" windowHeight="11580" xr2:uid="{176BBFA2-C1D9-4FD8-8B03-D771EE46934D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$256:$F$300</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="60">
   <si>
     <t>Thursday</t>
   </si>
@@ -175,12 +178,51 @@
   <si>
     <t>Trying to figure out how to send a mail via html</t>
   </si>
+  <si>
+    <t>cannelle</t>
+  </si>
+  <si>
+    <t>optional design</t>
+  </si>
+  <si>
+    <t>button background</t>
+  </si>
+  <si>
+    <t>HV</t>
+  </si>
+  <si>
+    <t>hv</t>
+  </si>
+  <si>
+    <t>cannellle</t>
+  </si>
+  <si>
+    <t>Cannelle hover buttons</t>
+  </si>
+  <si>
+    <t>cannell</t>
+  </si>
+  <si>
+    <t>regex to change links to links</t>
+  </si>
+  <si>
+    <t>CANNELLE</t>
+  </si>
+  <si>
+    <t>regex for french proverbs</t>
+  </si>
+  <si>
+    <t>thanks regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cannelle </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0\ &quot; m&quot;"/>
     <numFmt numFmtId="165" formatCode="0&quot;h&quot;"/>
@@ -188,6 +230,7 @@
     <numFmt numFmtId="167" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="168" formatCode="0&quot; m&quot;"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="172" formatCode="0.000\ &quot; m&quot;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -383,7 +426,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -490,16 +533,22 @@
     <xf numFmtId="168" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -820,16 +869,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA44BCE-BEAF-4B71-919F-0CAAC8D672FA}">
-  <dimension ref="A5:Z298"/>
+  <dimension ref="A5:Z497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B209" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C223" sqref="C223"/>
+    <sheetView tabSelected="1" topLeftCell="A299" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D322" sqref="D322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="13" customWidth="1"/>
     <col min="5" max="5" width="13" style="13" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="16" customWidth="1"/>
@@ -839,9 +888,11 @@
     <col min="10" max="10" width="9.140625" style="1"/>
     <col min="11" max="11" width="9.140625" style="2"/>
     <col min="12" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="12.85546875" style="1" customWidth="1"/>
-    <col min="15" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="13.28515625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="9.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" style="1" customWidth="1"/>
     <col min="20" max="23" width="9.140625" style="1"/>
     <col min="24" max="25" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="16384" width="9.140625" style="1"/>
@@ -857,13 +908,13 @@
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="4:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
     </row>
     <row r="15" spans="4:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
@@ -1493,7 +1544,7 @@
         <v>50.999999999999979</v>
       </c>
     </row>
-    <row r="69" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
         <v>15</v>
       </c>
@@ -1592,7 +1643,7 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="76" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C76" s="1" t="s">
         <v>15</v>
       </c>
@@ -2171,10 +2222,10 @@
         <f t="shared" si="2"/>
         <v>43.000000000000007</v>
       </c>
-      <c r="P113" s="37" t="s">
+      <c r="P113" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="Q113" s="37"/>
+      <c r="Q113" s="40"/>
     </row>
     <row r="114" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F114" s="16">
@@ -3383,7 +3434,7 @@
         <v>33.999999999999886</v>
       </c>
     </row>
-    <row r="178" spans="2:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="D178" s="13">
         <v>0.68263888888888891</v>
       </c>
@@ -3846,7 +3897,7 @@
       <c r="C209" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D209" s="38">
+      <c r="D209" s="36">
         <v>0.88402777777777775</v>
       </c>
       <c r="E209" s="13">
@@ -3995,7 +4046,7 @@
         <v>8</v>
       </c>
       <c r="I217" s="28">
-        <f>SUM(F217:F229)</f>
+        <f>SUM(F217:F223)</f>
         <v>371.99999999999977</v>
       </c>
       <c r="K217" s="30">
@@ -4127,7 +4178,7 @@
       <c r="R221" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S221" s="39">
+      <c r="S221" s="37">
         <f>P219/60*12</f>
         <v>134.1999999999999</v>
       </c>
@@ -4149,7 +4200,7 @@
       <c r="R222" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S222" s="39">
+      <c r="S222" s="37">
         <f>P219/60*15</f>
         <v>167.74999999999986</v>
       </c>
@@ -4175,451 +4226,2542 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B225" s="29">
+        <v>43841</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D225" s="13">
+        <v>0.60972222222222217</v>
+      </c>
+      <c r="E225" s="36">
+        <v>0.63958333333333328</v>
+      </c>
       <c r="F225" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="226" spans="6:6" x14ac:dyDescent="0.25">
+        <v>43.000000000000007</v>
+      </c>
+      <c r="H225" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I225" s="28">
+        <f>SUM(F225:F228)</f>
+        <v>285.99999999999994</v>
+      </c>
+      <c r="K225" s="30">
+        <f>(QUOTIENT(I225,60))</f>
+        <v>4</v>
+      </c>
+      <c r="L225" s="31">
+        <f>MOD(I225,60)</f>
+        <v>45.999999999999943</v>
+      </c>
+      <c r="O225" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P225" s="1">
+        <f>SUM($F$225:$F$228,$F$217:$F$222,$F$179:$F$180,$F$235,$F$238,$F$239)</f>
+        <v>924.99999999999966</v>
+      </c>
+      <c r="R225" s="30">
+        <f>(QUOTIENT(P225,60))</f>
+        <v>15</v>
+      </c>
+      <c r="S225" s="31">
+        <f>MOD(P225,60)</f>
+        <v>24.999999999999659</v>
+      </c>
+    </row>
+    <row r="226" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C226" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D226" s="13">
+        <v>0.64722222222222225</v>
+      </c>
+      <c r="E226" s="36">
+        <v>0.6645833333333333</v>
+      </c>
       <c r="F226" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="6:6" x14ac:dyDescent="0.25">
+        <v>24.999999999999911</v>
+      </c>
+    </row>
+    <row r="227" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C227" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D227" s="36">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="E227" s="36">
+        <v>0.77916666666666667</v>
+      </c>
       <c r="F227" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="6:6" x14ac:dyDescent="0.25">
+        <v>155.99999999999991</v>
+      </c>
+    </row>
+    <row r="228" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C228" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D228" s="13">
+        <v>0.87361111111111101</v>
+      </c>
+      <c r="E228" s="13">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="F228" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="6:6" x14ac:dyDescent="0.25">
+        <v>62.000000000000099</v>
+      </c>
+    </row>
+    <row r="229" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F229" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B230" s="29">
+        <v>43842</v>
+      </c>
+      <c r="D230" s="13">
+        <v>0.74583333333333324</v>
+      </c>
+      <c r="E230" s="13">
+        <v>0.75347222222222221</v>
+      </c>
       <c r="F230" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="6:6" x14ac:dyDescent="0.25">
+        <v>11.000000000000121</v>
+      </c>
+      <c r="H230" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I230" s="28">
+        <f>SUM(F230:F232)</f>
+        <v>53.000000000000121</v>
+      </c>
+      <c r="K230" s="30">
+        <f>(QUOTIENT(I230,60))</f>
+        <v>0</v>
+      </c>
+      <c r="L230" s="31">
+        <f>MOD(I230,60)</f>
+        <v>53.000000000000121</v>
+      </c>
+    </row>
+    <row r="231" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D231" s="13">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="E231" s="13">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="F231" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="6:6" x14ac:dyDescent="0.25">
+        <v>14.999999999999996</v>
+      </c>
+    </row>
+    <row r="232" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="C232" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D232" s="13">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E232" s="13">
+        <v>4.6527777777777779E-2</v>
+      </c>
       <c r="F232" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="6:6" x14ac:dyDescent="0.25">
+        <v>27.000000000000004</v>
+      </c>
+    </row>
+    <row r="233" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F233" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B234" s="29">
+        <v>43845</v>
+      </c>
+      <c r="D234" s="13">
+        <v>0.90763888888888899</v>
+      </c>
+      <c r="E234" s="13">
+        <v>0.91736111111111107</v>
+      </c>
       <c r="F234" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="6:6" x14ac:dyDescent="0.25">
+        <v>13.99999999999979</v>
+      </c>
+      <c r="H234" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I234" s="28">
+        <f>SUM(F234:F235)</f>
+        <v>57.999999999999787</v>
+      </c>
+      <c r="K234" s="30">
+        <f>(QUOTIENT(I234,60))</f>
+        <v>0</v>
+      </c>
+      <c r="L234" s="31">
+        <f>MOD(I234,60)</f>
+        <v>57.999999999999787</v>
+      </c>
+    </row>
+    <row r="235" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C235" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D235" s="13">
+        <v>0.91736111111111107</v>
+      </c>
+      <c r="E235" s="13">
+        <v>0.94791666666666663</v>
+      </c>
       <c r="F235" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F236" s="16">
-        <f t="shared" ref="F236:F298" si="6">(E236-D236)*24*60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F237" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="6:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="236" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D236" s="36"/>
+    </row>
+    <row r="238" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B238" s="29">
+        <v>43846</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D238" s="36">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="E238" s="13">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="F238" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F238:F239" si="6">(E238-D238)*24*60</f>
+        <v>48.000000000000071</v>
+      </c>
+      <c r="H238" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I238" s="28">
+        <f>SUM(F238:F240)</f>
+        <v>76.000000000000142</v>
+      </c>
+      <c r="K238" s="30">
+        <f>(QUOTIENT(I238,60))</f>
+        <v>1</v>
+      </c>
+      <c r="L238" s="31">
+        <f>MOD(I238,60)</f>
+        <v>16.000000000000142</v>
+      </c>
+      <c r="O238" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P238" s="1">
+        <f>SUM($F$225:$F$228,$F$217:$F$222,$F$179:$F$180,$F$235,$F$238,$F$239,$F$242,$F$248,$F$244,$F$249,$F$250)</f>
+        <v>993.99999999999955</v>
+      </c>
+      <c r="R238" s="30">
+        <f>(QUOTIENT(P238,60))</f>
+        <v>16</v>
+      </c>
+      <c r="S238" s="31">
+        <f>MOD(P238,60)</f>
+        <v>33.999999999999545</v>
+      </c>
+    </row>
+    <row r="239" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C239" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D239" s="13">
+        <v>0.52986111111111112</v>
+      </c>
+      <c r="E239" s="13">
+        <v>0.54722222222222217</v>
+      </c>
       <c r="F239" s="16">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="6:6" x14ac:dyDescent="0.25">
+        <v>24.999999999999911</v>
+      </c>
+    </row>
+    <row r="240" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D240" s="13">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E240" s="13">
+        <v>0.55069444444444449</v>
+      </c>
       <c r="F240" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F240:F303" si="7">(E240-D240)*24*60</f>
+        <v>3.0000000000001492</v>
+      </c>
+    </row>
+    <row r="241" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F241" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B242" s="29">
+        <v>43848</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D242" s="13">
+        <v>0.90902777777777777</v>
+      </c>
+      <c r="E242" s="13">
+        <v>0.92152777777777783</v>
+      </c>
       <c r="F242" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>18.000000000000096</v>
+      </c>
+      <c r="H242" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I242" s="28">
+        <f>SUM(F242)</f>
+        <v>18.000000000000096</v>
+      </c>
+      <c r="K242" s="30">
+        <f>(QUOTIENT(I242,60))</f>
+        <v>0</v>
+      </c>
+      <c r="L242" s="31">
+        <f>MOD(I242,60)</f>
+        <v>18.000000000000096</v>
+      </c>
+    </row>
+    <row r="243" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F243" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B244" s="29">
+        <v>43849</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D244" s="13">
+        <v>0.51666666666666672</v>
+      </c>
+      <c r="E244" s="13">
+        <v>0.5229166666666667</v>
+      </c>
       <c r="F244" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>8.999999999999968</v>
+      </c>
+      <c r="H244" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I244" s="28">
+        <f>SUM(F244:F258)</f>
+        <v>197.99999999999994</v>
+      </c>
+      <c r="K244" s="30">
+        <f>(QUOTIENT(I244,60))</f>
+        <v>3</v>
+      </c>
+      <c r="L244" s="31">
+        <f>MOD(I244,60)</f>
+        <v>17.999999999999943</v>
+      </c>
+    </row>
+    <row r="245" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="C245" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D245" s="36">
+        <v>4.1666666666666666E-3</v>
+      </c>
       <c r="F245" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="246" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F246" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B247" s="29">
+        <v>43850</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D247" s="13">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="E247" s="13">
+        <v>0.77916666666666667</v>
+      </c>
       <c r="F247" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>79.000000000000043</v>
+      </c>
+      <c r="H247" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I247" s="28">
+        <f>SUM(F247:F254)</f>
+        <v>172.99999999999989</v>
+      </c>
+      <c r="K247" s="30">
+        <f>(QUOTIENT(I247,60))</f>
+        <v>2</v>
+      </c>
+      <c r="L247" s="31">
+        <f>MOD(I247,60)</f>
+        <v>52.999999999999886</v>
+      </c>
+    </row>
+    <row r="248" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C248" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D248" s="13">
+        <v>0.75694444444444453</v>
+      </c>
+      <c r="E248" s="13">
+        <v>0.77916666666666667</v>
+      </c>
       <c r="F248" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>31.999999999999886</v>
+      </c>
+    </row>
+    <row r="249" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C249" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D249" s="13">
+        <v>0.78263888888888899</v>
+      </c>
+      <c r="E249" s="13">
+        <v>0.78333333333333333</v>
+      </c>
       <c r="F249" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0.99999999999983658</v>
+      </c>
+    </row>
+    <row r="250" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C250" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D250" s="13">
+        <v>0.78333333333333333</v>
+      </c>
+      <c r="E250" s="13">
+        <v>0.7895833333333333</v>
+      </c>
       <c r="F250" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>8.999999999999968</v>
+      </c>
+    </row>
+    <row r="251" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C251" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D251" s="13">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E251" s="36">
+        <v>0.80555555555555547</v>
+      </c>
       <c r="F251" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>19.999999999999929</v>
+      </c>
+    </row>
+    <row r="252" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C252" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D252" s="13">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="E252" s="13">
+        <v>0.83611111111111114</v>
+      </c>
       <c r="F252" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>14.00000000000011</v>
+      </c>
+    </row>
+    <row r="253" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C253" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D253" s="13">
+        <v>0.84166666666666667</v>
+      </c>
+      <c r="E253" s="13">
+        <v>0.84305555555555556</v>
+      </c>
       <c r="F253" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>1.9999999999999929</v>
+      </c>
+    </row>
+    <row r="254" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C254" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D254" s="13">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E254" s="36">
+        <v>0.85833333333333339</v>
+      </c>
       <c r="F254" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F255" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>16.000000000000103</v>
+      </c>
+    </row>
+    <row r="255" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E255" s="36"/>
+    </row>
+    <row r="256" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B256" s="29">
+        <v>43851</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D256" s="13">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="E256" s="13">
+        <v>0.60069444444444442</v>
+      </c>
       <c r="F256" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>4.9999999999999822</v>
+      </c>
+      <c r="H256" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I256" s="28">
+        <f>SUM(F256:F264)</f>
+        <v>154.00000000000026</v>
+      </c>
+      <c r="K256" s="30">
+        <f>(QUOTIENT(I256,60))</f>
+        <v>2</v>
+      </c>
+      <c r="L256" s="31">
+        <f>MOD(I256,60)</f>
+        <v>34.000000000000256</v>
+      </c>
+    </row>
+    <row r="257" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D257" s="13">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="E257" s="13">
+        <v>0.60763888888888895</v>
+      </c>
       <c r="F257" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>10.000000000000124</v>
+      </c>
+    </row>
+    <row r="258" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="D258" s="36">
+        <v>0.65416666666666667</v>
+      </c>
+      <c r="E258" s="13">
+        <v>0.65902777777777777</v>
+      </c>
       <c r="F258" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>6.9999999999999751</v>
+      </c>
+      <c r="O258" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P258" s="1">
+        <f>SUM($F$225:$F$228,$F$217:$F$222,$F$179:$F$180,$F$235,$F$238,$F$239,$F$242,$F$248,$F$244,$F$249,$F$250,$F$256)</f>
+        <v>998.99999999999955</v>
+      </c>
+      <c r="R258" s="30">
+        <f>(QUOTIENT(P258,60))</f>
+        <v>16</v>
+      </c>
+      <c r="S258" s="31">
+        <f>MOD(P258,60)</f>
+        <v>38.999999999999545</v>
+      </c>
+    </row>
+    <row r="259" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D259" s="13">
+        <v>0.66111111111111109</v>
+      </c>
+      <c r="E259" s="36">
+        <v>0.67291666666666661</v>
+      </c>
       <c r="F259" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>16.99999999999994</v>
+      </c>
+    </row>
+    <row r="260" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D260" s="13">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="E260" s="13">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="F260" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>30.000000000000053</v>
+      </c>
+    </row>
+    <row r="261" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D261" s="13">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="E261" s="13">
+        <v>0.71111111111111114</v>
+      </c>
       <c r="F261" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>14.00000000000011</v>
+      </c>
+    </row>
+    <row r="262" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D262" s="13">
+        <v>0.72638888888888886</v>
+      </c>
+      <c r="E262" s="13">
+        <v>0.74097222222222225</v>
+      </c>
       <c r="F262" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>21.000000000000085</v>
+      </c>
+    </row>
+    <row r="263" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D263" s="36">
+        <v>0.78055555555555556</v>
+      </c>
+      <c r="E263" s="13">
+        <v>0.78263888888888899</v>
+      </c>
       <c r="F263" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>3.0000000000001492</v>
+      </c>
+    </row>
+    <row r="264" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D264" s="36">
+        <v>0.79375000000000007</v>
+      </c>
+      <c r="E264" s="13">
+        <v>0.82638888888888884</v>
+      </c>
       <c r="F264" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="265" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>46.999999999999829</v>
+      </c>
+    </row>
+    <row r="265" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F265" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B266" s="29">
+        <v>43852</v>
+      </c>
+      <c r="D266" s="13">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="E266" s="36">
+        <v>0.34097222222222223</v>
+      </c>
       <c r="F266" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="267" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>36.000000000000028</v>
+      </c>
+      <c r="H266" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I266" s="28">
+        <f>SUM(F266:F280)</f>
+        <v>496.00000000000017</v>
+      </c>
+      <c r="K266" s="30">
+        <f>(QUOTIENT(I266,60))</f>
+        <v>8</v>
+      </c>
+      <c r="L266" s="31">
+        <f>MOD(I266,60)</f>
+        <v>16.000000000000171</v>
+      </c>
+    </row>
+    <row r="267" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D267" s="36">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E267" s="13">
+        <v>0.35902777777777778</v>
+      </c>
       <c r="F267" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>6.9999999999999751</v>
+      </c>
+    </row>
+    <row r="268" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D268" s="36">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="E268" s="36">
+        <v>0.41250000000000003</v>
+      </c>
       <c r="F268" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>14.00000000000011</v>
+      </c>
+    </row>
+    <row r="269" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D269" s="13">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="E269" s="13">
+        <v>0.4284722222222222</v>
+      </c>
       <c r="F269" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>11.999999999999957</v>
+      </c>
+    </row>
+    <row r="270" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D270" s="36">
+        <v>0.45694444444444443</v>
+      </c>
+      <c r="E270" s="36">
+        <v>0.48888888888888887</v>
+      </c>
       <c r="F270" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="271" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="C271" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D271" s="36">
+        <v>0.51597222222222217</v>
+      </c>
+      <c r="E271" s="13">
+        <v>0.53125</v>
+      </c>
       <c r="F271" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="272" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>22.000000000000082</v>
+      </c>
+    </row>
+    <row r="272" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C272" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D272" s="13">
+        <v>0.55486111111111114</v>
+      </c>
+      <c r="E272" s="13">
+        <v>0.5625</v>
+      </c>
       <c r="F272" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="273" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>10.999999999999961</v>
+      </c>
+    </row>
+    <row r="273" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C273" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D273" s="36">
+        <v>0.65833333333333333</v>
+      </c>
+      <c r="E273" s="36">
+        <v>0.67569444444444438</v>
+      </c>
       <c r="F273" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="274" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>24.999999999999911</v>
+      </c>
+    </row>
+    <row r="274" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="C274" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D274" s="13">
+        <v>0.67569444444444438</v>
+      </c>
+      <c r="E274" s="36">
+        <v>0.7055555555555556</v>
+      </c>
       <c r="F274" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>43.000000000000171</v>
+      </c>
+      <c r="N274" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O274" s="1">
+        <f>SUM($F$225:$F$228,$F$217:$F$222,$F$179:$F$180,$F$235,$F$238,$F$239,$F$242,$F$248,$F$244,$F$249,$F$250,$F$256,$F$275,$F$273,$F$272,$F$277,$F$279, $F$283,$F$282,$F$284,$F$286)</f>
+        <v>1357.9999999999995</v>
+      </c>
+      <c r="Q274" s="30">
+        <f>(QUOTIENT(O274,60))</f>
+        <v>22</v>
+      </c>
+      <c r="R274" s="31">
+        <f>MOD(O274,60)</f>
+        <v>37.999999999999545</v>
+      </c>
+    </row>
+    <row r="275" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C275" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D275" s="13">
+        <v>0.7055555555555556</v>
+      </c>
+      <c r="E275" s="13">
+        <v>0.7319444444444444</v>
+      </c>
       <c r="F275" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="276" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>37.999999999999865</v>
+      </c>
+    </row>
+    <row r="276" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F276" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B277" s="29">
+        <v>43853</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D277" s="13">
+        <v>0.39861111111111108</v>
+      </c>
+      <c r="E277" s="13">
+        <v>0.41250000000000003</v>
+      </c>
       <c r="F277" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="278" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>20.000000000000089</v>
+      </c>
+    </row>
+    <row r="278" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="C278" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D278" s="13">
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="E278" s="13">
+        <v>0.49583333333333335</v>
+      </c>
       <c r="F278" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="279" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>119.99999999999997</v>
+      </c>
+    </row>
+    <row r="279" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C279" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D279" s="13">
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="E279" s="13">
+        <v>0.52500000000000002</v>
+      </c>
       <c r="F279" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="280" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>52.000000000000057</v>
+      </c>
+    </row>
+    <row r="280" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C280" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D280" s="36">
+        <v>0.65625</v>
+      </c>
+      <c r="E280" s="13">
+        <v>0.69097222222222221</v>
+      </c>
       <c r="F280" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="281" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>49.999999999999986</v>
+      </c>
+    </row>
+    <row r="281" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D281" s="38"/>
       <c r="F281" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C282" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D282" s="36">
+        <v>0.59375</v>
+      </c>
+      <c r="E282" s="13">
+        <v>0.65763888888888888</v>
+      </c>
       <c r="F282" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="283" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B283" s="29">
+        <v>43854</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D283" s="36">
+        <v>0.74652777777777779</v>
+      </c>
+      <c r="E283" s="13">
+        <v>0.8125</v>
+      </c>
       <c r="F283" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>94.999999999999986</v>
+      </c>
+    </row>
+    <row r="284" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C284" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D284" s="13">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="E284" s="13">
+        <v>0.9375</v>
+      </c>
       <c r="F284" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="285" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>10.000000000000124</v>
+      </c>
+    </row>
+    <row r="285" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F285" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="286" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B286" s="29">
+        <v>43855</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D286" s="13">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E286" s="13">
+        <v>0.65694444444444444</v>
+      </c>
       <c r="F286" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>15.999999999999943</v>
+      </c>
+    </row>
+    <row r="287" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D287" s="13">
+        <v>0.65763888888888888</v>
+      </c>
+      <c r="E287" s="13">
+        <v>0.67499999999999993</v>
+      </c>
       <c r="F287" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>24.999999999999911</v>
+      </c>
+    </row>
+    <row r="288" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F288" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B289" s="29">
+        <v>43857</v>
+      </c>
+      <c r="D289" s="36">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="E289" s="13">
+        <v>0.33888888888888885</v>
+      </c>
       <c r="F289" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>17.999999999999936</v>
+      </c>
+      <c r="H289" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I289" s="28">
+        <f>SUM(F289:F291)</f>
+        <v>66</v>
+      </c>
+      <c r="K289" s="30">
+        <f>(QUOTIENT(I289,60))</f>
+        <v>1</v>
+      </c>
+      <c r="L289" s="31">
+        <f>MOD(I289,60)</f>
+        <v>6</v>
+      </c>
+      <c r="N289" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O289" s="1">
+        <f>SUM($F$225:$F$228,$F$217:$F$222,$F$179:$F$180,$F$235,$F$238,$F$301,$F$300,$F$297,$F$298,$F$293,$F$295,$F$239,$F$242,$F$248,$F$244,$F$249,$F$250,$F$256,$F$275,$F$273,$F$272,$F$277,$F$279, $F$283,$F$282,$F$284,$F$286)</f>
+        <v>1624.9999999999993</v>
+      </c>
+      <c r="Q289" s="30">
+        <f>(QUOTIENT(O289,60))</f>
+        <v>27</v>
+      </c>
+      <c r="R289" s="31">
+        <f>MOD(O289,60)</f>
+        <v>4.9999999999993179</v>
+      </c>
+    </row>
+    <row r="290" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D290" s="13">
+        <v>0.3743055555555555</v>
+      </c>
+      <c r="E290" s="13">
+        <v>0.39027777777777778</v>
+      </c>
       <c r="F290" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="291" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>23.000000000000078</v>
+      </c>
+    </row>
+    <row r="291" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D291" s="13">
+        <v>0.40347222222222223</v>
+      </c>
+      <c r="E291" s="13">
+        <v>0.42083333333333334</v>
+      </c>
       <c r="F291" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>24.999999999999993</v>
+      </c>
+    </row>
+    <row r="292" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F292" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B293" s="29">
+        <v>43857</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D293" s="13">
+        <v>0.7416666666666667</v>
+      </c>
+      <c r="E293" s="13">
+        <v>0.75347222222222221</v>
+      </c>
       <c r="F293" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>16.99999999999994</v>
+      </c>
+    </row>
+    <row r="294" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F294" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="295" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B295" s="29">
+        <v>43858</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D295" s="13">
+        <v>0.65347222222222223</v>
+      </c>
+      <c r="E295" s="36">
+        <v>0.65833333333333333</v>
+      </c>
       <c r="F295" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="296" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>6.9999999999999751</v>
+      </c>
+    </row>
+    <row r="296" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C296" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D296" s="13">
+        <v>0.65833333333333333</v>
+      </c>
+      <c r="E296" s="13">
+        <v>0.69097222222222221</v>
+      </c>
       <c r="F296" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>46.999999999999993</v>
+      </c>
+    </row>
+    <row r="297" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C297" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D297" s="13">
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="E297" s="13">
+        <v>0.70277777777777783</v>
+      </c>
       <c r="F297" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="298" spans="6:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>27.000000000000064</v>
+      </c>
+    </row>
+    <row r="298" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C298" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D298" s="13">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="E298" s="13">
+        <v>0.77638888888888891</v>
+      </c>
       <c r="F298" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v>102.99999999999996</v>
+      </c>
+    </row>
+    <row r="299" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F299" s="16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B300" s="29">
+        <v>43860</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D300" s="13">
+        <v>0.46875</v>
+      </c>
+      <c r="E300" s="13">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="F300" s="16">
+        <f t="shared" si="7"/>
+        <v>13.000000000000034</v>
+      </c>
+    </row>
+    <row r="301" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C301" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D301" s="13">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="E301" s="13">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="F301" s="16">
+        <f t="shared" si="7"/>
+        <v>99.999999999999801</v>
+      </c>
+    </row>
+    <row r="302" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C302" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D302" s="13">
+        <v>0.88055555555555554</v>
+      </c>
+      <c r="E302" s="13">
+        <v>0.89930555555555547</v>
+      </c>
+      <c r="F302" s="16">
+        <f t="shared" si="7"/>
+        <v>26.999999999999904</v>
+      </c>
+    </row>
+    <row r="303" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="C303" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D303" s="13">
+        <v>0.90625</v>
+      </c>
+      <c r="E303" s="13">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="F303" s="16">
+        <f t="shared" si="7"/>
+        <v>10.000000000000124</v>
+      </c>
+      <c r="N303" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O303" s="1">
+        <f>SUM($F$225:$F$228,$F$302,$F$303,$F$305,$F$217:$F$222,$F$179:$F$180,$F$235,$F$238,$F$301,$F$306,$F$300,$F$297,$F$298,$F$293,$F$295,$F$239,$F$242,$F$248,$F$244,$F$249,$F$250,$F$256,$F$275,$F$273,$F$272,$F$277,$F$279, $F$283,$F$282,$F$284,$F$286)</f>
+        <v>1831.9999999999993</v>
+      </c>
+      <c r="Q303" s="30">
+        <f>(QUOTIENT(O303,60))</f>
+        <v>30</v>
+      </c>
+      <c r="R303" s="31">
+        <f>MOD(O303,60)</f>
+        <v>31.999999999999318</v>
+      </c>
+    </row>
+    <row r="304" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F304" s="16">
+        <f t="shared" ref="F304:F367" si="8">(E304-D304)*24*60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B305" s="29">
+        <v>43861</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D305" s="13">
+        <v>0.93819444444444444</v>
+      </c>
+      <c r="E305" s="13">
+        <v>0.99375000000000002</v>
+      </c>
+      <c r="F305" s="16">
+        <f t="shared" si="8"/>
+        <v>80.000000000000028</v>
+      </c>
+    </row>
+    <row r="306" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C306" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D306" s="13">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E306" s="13">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="F306" s="16">
+        <f t="shared" si="8"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="307" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F307" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B308" s="29">
+        <v>43866</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D308" s="13">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="E308" s="13">
+        <v>0.7944444444444444</v>
+      </c>
+      <c r="F308" s="16">
+        <f t="shared" si="8"/>
+        <v>42.999999999999844</v>
+      </c>
+    </row>
+    <row r="309" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F309" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I309" s="41"/>
+    </row>
+    <row r="310" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B310" s="29">
+        <v>43867</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D310" s="13">
+        <v>0.4375</v>
+      </c>
+      <c r="E310" s="13">
+        <v>0.46388888888888885</v>
+      </c>
+      <c r="F310" s="16">
+        <f t="shared" si="8"/>
+        <v>37.999999999999943</v>
+      </c>
+      <c r="H310" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I310" s="28">
+        <f>SUM(F310:F325)</f>
+        <v>-627.00000000000023</v>
+      </c>
+      <c r="K310" s="30">
+        <f>(QUOTIENT(I310,60))</f>
+        <v>-10</v>
+      </c>
+      <c r="L310" s="31">
+        <f>MOD(I310,60)</f>
+        <v>32.999999999999773</v>
+      </c>
+    </row>
+    <row r="311" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D311" s="36">
+        <v>0.50624999999999998</v>
+      </c>
+      <c r="E311" s="13">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F311" s="16">
+        <f t="shared" si="8"/>
+        <v>21.000000000000085</v>
+      </c>
+    </row>
+    <row r="312" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D312" s="13">
+        <v>0.59375</v>
+      </c>
+      <c r="E312" s="13">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="F312" s="16">
+        <f t="shared" si="8"/>
+        <v>126.00000000000003</v>
+      </c>
+    </row>
+    <row r="313" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D313" s="36">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="E313" s="13">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="F313" s="16">
+        <f t="shared" si="8"/>
+        <v>26.999999999999904</v>
+      </c>
+    </row>
+    <row r="314" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D314" s="36">
+        <v>0.8354166666666667</v>
+      </c>
+      <c r="E314" s="13">
+        <v>0.87013888888888891</v>
+      </c>
+      <c r="F314" s="16">
+        <f t="shared" si="8"/>
+        <v>49.999999999999986</v>
+      </c>
+    </row>
+    <row r="315" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F315" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D316" s="36">
+        <v>0.33958333333333335</v>
+      </c>
+      <c r="E316" s="13">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="F316" s="16">
+        <f t="shared" si="8"/>
+        <v>26.999999999999986</v>
+      </c>
+    </row>
+    <row r="317" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D317" s="13">
+        <v>0.36736111111111108</v>
+      </c>
+      <c r="E317" s="13">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F317" s="16">
+        <f t="shared" si="8"/>
+        <v>41.000000000000014</v>
+      </c>
+    </row>
+    <row r="318" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D318" s="13">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E318" s="13">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="F318" s="16">
+        <f t="shared" si="8"/>
+        <v>4.9999999999999822</v>
+      </c>
+    </row>
+    <row r="319" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D319" s="13">
+        <v>0.4381944444444445</v>
+      </c>
+      <c r="E319" s="13">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="F319" s="16">
+        <f t="shared" si="8"/>
+        <v>67.999999999999915</v>
+      </c>
+    </row>
+    <row r="320" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D320" s="13">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E320" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F320" s="16">
+        <f t="shared" si="8"/>
+        <v>69.999999999999915</v>
+      </c>
+    </row>
+    <row r="321" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D321" s="13">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="F321" s="16">
+        <f t="shared" si="8"/>
+        <v>-1100</v>
+      </c>
+    </row>
+    <row r="322" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F322" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F323" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F324" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F325" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F326" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F327" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F328" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F329" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F330" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F331" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F332" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F333" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F334" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F335" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F336" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F337" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F338" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F339" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F340" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F341" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F342" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F343" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F344" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F345" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F346" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F347" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F348" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F349" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F350" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F351" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F352" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F353" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F354" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F355" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F356" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F357" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F358" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F359" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F360" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F361" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F362" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F363" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F364" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F365" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F366" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F367" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F368" s="16">
+        <f t="shared" ref="F368:F431" si="9">(E368-D368)*24*60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F369" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F370" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F371" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F372" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F373" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F374" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F375" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F376" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F377" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F378" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F379" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F380" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F381" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F382" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F383" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F384" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F385" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F386" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F387" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F388" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F389" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F390" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F391" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F392" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F393" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F394" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F395" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F396" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F397" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F398" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F399" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="400" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F400" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F401" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F402" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F403" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F404" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F405" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F406" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F407" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F408" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F409" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F410" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F411" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F412" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F413" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F414" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F415" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F416" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F417" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F418" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F419" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F420" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F421" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F422" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F423" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F424" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F425" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F426" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F427" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F428" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F429" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F430" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F431" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F432" s="16">
+        <f t="shared" ref="F432:F495" si="10">(E432-D432)*24*60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F433" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F434" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F435" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F436" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F437" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F438" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F439" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F440" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F441" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="442" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F442" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F443" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F444" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F445" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F446" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F447" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F448" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F449" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F450" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F451" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F452" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F453" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F454" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F455" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F456" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F457" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F458" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F459" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F460" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F461" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F462" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F463" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F464" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F465" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F466" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F467" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F468" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F469" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="470" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F470" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="471" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F471" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F472" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F473" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F474" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F475" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F476" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F477" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F478" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="479" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F479" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F480" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F481" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F482" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F483" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F484" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F485" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F486" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F487" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F488" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="489" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F489" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F490" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F491" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F492" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F493" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="494" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F494" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F495" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F496" s="16">
+        <f t="shared" ref="F496:F497" si="11">(E496-D496)*24*60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F497" s="16">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B256:F300" xr:uid="{C8B3E621-0270-49BB-B482-FD2982FD38D7}"/>
   <mergeCells count="2">
     <mergeCell ref="F14:J14"/>
     <mergeCell ref="P113:Q113"/>

</xml_diff>